<commit_message>
testing and final clean up
</commit_message>
<xml_diff>
--- a/Team_Charter_Grid.xlsx
+++ b/Team_Charter_Grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganda\Documents\GitHub\Software-Engineering-Principles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB035B6-00EE-499E-9C87-170889D41689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD6AC1-FE90-410D-AE13-7398C1BE4795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93A11A4B-CEF3-43A0-97C9-7F2E05BB152B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93A11A4B-CEF3-43A0-97C9-7F2E05BB152B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -258,25 +258,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -596,7 +596,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10:M10"/>
+      <selection activeCell="D18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -607,95 +607,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
       <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15" t="s">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15" t="s">
+      <c r="K3" s="13"/>
+      <c r="L3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15" t="s">
+      <c r="M3" s="13"/>
+      <c r="N3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15" t="s">
+      <c r="O3" s="13"/>
+      <c r="P3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="15"/>
+      <c r="Q3" s="13"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -722,27 +722,27 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="12">
         <v>1</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" s="10">
+      <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="10">
+      <c r="F5" s="12">
         <v>0</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="10">
+      <c r="H5" s="12">
         <v>0</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="10">
+      <c r="J5" s="12">
         <v>0</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="10">
+      <c r="L5" s="12">
         <v>0</v>
       </c>
       <c r="M5" s="9"/>
@@ -755,27 +755,27 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="12">
         <v>0</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="10">
+      <c r="F6" s="12">
         <v>1</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="10">
+      <c r="H6" s="12">
         <v>1</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="10">
+      <c r="J6" s="12">
         <v>0</v>
       </c>
       <c r="K6" s="9"/>
-      <c r="L6" s="10">
+      <c r="L6" s="12">
         <v>0</v>
       </c>
       <c r="M6" s="9"/>
@@ -788,27 +788,27 @@
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="12">
         <v>1</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>1</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="10">
+      <c r="F7" s="12">
         <v>0</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="10">
+      <c r="H7" s="12">
         <v>0</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="10">
+      <c r="J7" s="12">
         <v>0</v>
       </c>
       <c r="K7" s="9"/>
-      <c r="L7" s="10">
+      <c r="L7" s="12">
         <v>0</v>
       </c>
       <c r="M7" s="9"/>
@@ -821,28 +821,28 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="12">
         <v>0.33</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="10">
-        <v>0.25</v>
+      <c r="D8" s="12">
+        <v>0.2</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="10">
+      <c r="F8" s="12">
         <v>0.33</v>
       </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="10">
+      <c r="H8" s="12">
         <v>0</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="10">
+      <c r="J8" s="12">
         <v>0.33</v>
       </c>
       <c r="K8" s="9"/>
-      <c r="L8" s="10">
-        <v>0.75</v>
+      <c r="L8" s="12">
+        <v>0.8</v>
       </c>
       <c r="M8" s="9"/>
       <c r="N8" s="8"/>
@@ -875,27 +875,27 @@
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="12">
         <v>0.33</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <v>1</v>
       </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="10">
+      <c r="F10" s="12">
         <v>0.33</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="10">
+      <c r="H10" s="12">
         <v>0</v>
       </c>
       <c r="I10" s="9"/>
-      <c r="J10" s="10">
+      <c r="J10" s="12">
         <v>0.33</v>
       </c>
       <c r="K10" s="9"/>
-      <c r="L10" s="10">
+      <c r="L10" s="12">
         <v>0</v>
       </c>
       <c r="M10" s="9"/>
@@ -908,27 +908,27 @@
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="12">
         <v>0.33</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="10">
+      <c r="D11" s="12">
         <v>0.8</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="10">
+      <c r="F11" s="12">
         <v>0.33</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="10">
+      <c r="H11" s="12">
         <v>0</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="10">
+      <c r="J11" s="12">
         <v>0.33</v>
       </c>
       <c r="K11" s="9"/>
-      <c r="L11" s="10">
+      <c r="L11" s="12">
         <v>0.2</v>
       </c>
       <c r="M11" s="9"/>
@@ -941,27 +941,27 @@
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="12">
         <v>0</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="10">
+      <c r="D12" s="12">
         <v>0</v>
       </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="10">
+      <c r="F12" s="12">
         <v>0</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="10">
+      <c r="H12" s="12">
         <v>0</v>
       </c>
       <c r="I12" s="9"/>
-      <c r="J12" s="10">
+      <c r="J12" s="12">
         <v>1</v>
       </c>
       <c r="K12" s="9"/>
-      <c r="L12" s="10">
+      <c r="L12" s="12">
         <v>1</v>
       </c>
       <c r="M12" s="9"/>
@@ -974,27 +974,27 @@
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="12">
         <v>0</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="10">
+      <c r="D13" s="12">
         <v>0</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="10">
+      <c r="F13" s="12">
         <v>0</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="10">
+      <c r="H13" s="12">
         <v>1</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="10">
+      <c r="J13" s="12">
         <v>1</v>
       </c>
       <c r="K13" s="9"/>
-      <c r="L13" s="10">
+      <c r="L13" s="12">
         <v>0</v>
       </c>
       <c r="M13" s="9"/>
@@ -1007,27 +1007,27 @@
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="12">
         <v>0</v>
       </c>
       <c r="C14" s="9"/>
-      <c r="D14" s="10">
+      <c r="D14" s="12">
         <v>0</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="10">
+      <c r="F14" s="12">
         <v>0</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="10">
+      <c r="H14" s="12">
         <v>0</v>
       </c>
       <c r="I14" s="9"/>
-      <c r="J14" s="10">
+      <c r="J14" s="12">
         <v>1</v>
       </c>
       <c r="K14" s="9"/>
-      <c r="L14" s="10">
+      <c r="L14" s="12">
         <v>1</v>
       </c>
       <c r="M14" s="9"/>
@@ -1040,27 +1040,27 @@
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="12">
         <v>1</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="10">
+      <c r="D15" s="12">
         <v>1</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="10">
+      <c r="F15" s="12">
         <v>0</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="10">
+      <c r="H15" s="12">
         <v>0</v>
       </c>
       <c r="I15" s="9"/>
-      <c r="J15" s="10">
+      <c r="J15" s="12">
         <v>0</v>
       </c>
       <c r="K15" s="9"/>
-      <c r="L15" s="10">
+      <c r="L15" s="12">
         <v>0</v>
       </c>
       <c r="M15" s="9"/>
@@ -1073,27 +1073,27 @@
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="12">
         <v>0</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="10">
+      <c r="D16" s="12">
         <v>0</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="10">
+      <c r="F16" s="12">
         <v>1</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="10">
+      <c r="H16" s="12">
         <v>1</v>
       </c>
       <c r="I16" s="9"/>
-      <c r="J16" s="10">
+      <c r="J16" s="12">
         <v>0</v>
       </c>
       <c r="K16" s="9"/>
-      <c r="L16" s="10">
+      <c r="L16" s="12">
         <v>0</v>
       </c>
       <c r="M16" s="9"/>
@@ -1106,27 +1106,27 @@
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="12">
         <v>1</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="10">
+      <c r="D17" s="12">
         <v>1</v>
       </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="10">
+      <c r="F17" s="12">
         <v>0</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="10">
+      <c r="H17" s="12">
         <v>0</v>
       </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="10">
+      <c r="J17" s="12">
         <v>0</v>
       </c>
       <c r="K17" s="9"/>
-      <c r="L17" s="10">
+      <c r="L17" s="12">
         <v>0</v>
       </c>
       <c r="M17" s="9"/>
@@ -1139,27 +1139,27 @@
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="12">
         <v>0.33</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="10">
+      <c r="D18" s="12">
         <v>1</v>
       </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="10">
+      <c r="F18" s="12">
         <v>0.33</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="10">
+      <c r="H18" s="12">
         <v>0</v>
       </c>
       <c r="I18" s="9"/>
-      <c r="J18" s="10">
+      <c r="J18" s="12">
         <v>0.33</v>
       </c>
       <c r="K18" s="9"/>
-      <c r="L18" s="10">
+      <c r="L18" s="12">
         <v>0</v>
       </c>
       <c r="M18" s="9"/>
@@ -1172,82 +1172,188 @@
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="15">
         <f>SUM(B5,B6,B7,B8,B10,B11,B12,B13,B14,B15, B16,B17,B18)</f>
         <v>5.32</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16">
         <f t="shared" ref="D19" si="0">SUM(D5,D6,D7,D8,D10,D11,D12,D13,D14,D15, D16,D17,D18)</f>
-        <v>7.05</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12">
+        <v>7</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16">
         <f t="shared" ref="F19" si="1">SUM(F5,F6,F7,F8,F10,F11,F12,F13,F14,F15, F16,F17,F18)</f>
         <v>3.3200000000000003</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12">
+      <c r="G19" s="16"/>
+      <c r="H19" s="16">
         <f t="shared" ref="H19" si="2">SUM(H5,H6,H7,H8,H10,H11,H12,H13,H14,H15, H16,H17,H18)</f>
         <v>3</v>
       </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12">
+      <c r="I19" s="16"/>
+      <c r="J19" s="16">
         <f t="shared" ref="J19" si="3">SUM(J5,J6,J7,J8,J10,J11,J12,J13,J14,J15, J16,J17,J18)</f>
         <v>4.32</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12">
+      <c r="K19" s="16"/>
+      <c r="L19" s="16">
         <f t="shared" ref="L19" si="4">SUM(L5,L6,L7,L8,L10,L11,L12,L13,L14,L15, L16,L17,L18)</f>
-        <v>2.95</v>
-      </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12">
+        <v>3</v>
+      </c>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16">
         <f t="shared" ref="N19" si="5">SUM(N5,N6,N7,N8,N10,N11,N12,N13,N14,N15, N16,N17,N18)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12">
+      <c r="O19" s="16"/>
+      <c r="P19" s="16">
         <f t="shared" ref="P19" si="6">SUM(P5,P6,P7,P8,P10,P11,P12,P13,P14,P15, P16,P17,P18)</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="12"/>
+      <c r="Q19" s="16"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="14">
         <f>SUM(B19-D19)</f>
-        <v>-1.7299999999999995</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11">
+        <v>-1.6799999999999997</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14">
         <f t="shared" ref="F20" si="7">SUM(F19-H19)</f>
         <v>0.32000000000000028</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11">
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14">
         <f t="shared" ref="J20" si="8">SUM(J19-L19)</f>
-        <v>1.37</v>
-      </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11">
+        <v>1.3200000000000003</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14">
         <f t="shared" ref="N20" si="9">SUM(N19-P19)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="130">
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="P15:Q15"/>
     <mergeCell ref="B1:Q1"/>
     <mergeCell ref="A1:A3"/>
@@ -1272,112 +1378,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
design documentation writeup complete
</commit_message>
<xml_diff>
--- a/Team_Charter_Grid.xlsx
+++ b/Team_Charter_Grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganda\Documents\GitHub\Software-Engineering-Principles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD6AC1-FE90-410D-AE13-7398C1BE4795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6444A2B8-6D50-4A1F-A556-DE090E242535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93A11A4B-CEF3-43A0-97C9-7F2E05BB152B}"/>
   </bookViews>
@@ -596,7 +596,7 @@
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E18"/>
+      <selection activeCell="H6" sqref="H6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="12">
@@ -768,7 +768,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="12">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="12">
@@ -1179,7 +1179,7 @@
       <c r="C19" s="16"/>
       <c r="D19" s="16">
         <f t="shared" ref="D19" si="0">SUM(D5,D6,D7,D8,D10,D11,D12,D13,D14,D15, D16,D17,D18)</f>
-        <v>7</v>
+        <v>7.3</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16">
@@ -1189,7 +1189,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="16">
         <f t="shared" ref="H19" si="2">SUM(H5,H6,H7,H8,H10,H11,H12,H13,H14,H15, H16,H17,H18)</f>
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="16">
@@ -1219,14 +1219,14 @@
       </c>
       <c r="B20" s="14">
         <f>SUM(B19-D19)</f>
-        <v>-1.6799999999999997</v>
+        <v>-1.9799999999999995</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14">
         <f t="shared" ref="F20" si="7">SUM(F19-H19)</f>
-        <v>0.32000000000000028</v>
+        <v>0.62000000000000011</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>

</xml_diff>